<commit_message>
update content and Style
</commit_message>
<xml_diff>
--- a/docs/aussteller.xlsx
+++ b/docs/aussteller.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Veranstaltungen\Deutscher Tourismustag\DTT_2014_Freiburg\App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Veranstaltungen\Deutscher Tourismustag\DTT_2014_Freiburg\App MobileSeite\Aussteller\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Messe Essen GmbH</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name Aussteller</t>
   </si>
@@ -36,23 +33,56 @@
     <t>Kampmann GmbH - international</t>
   </si>
   <si>
-    <t>Europäische Reiseversicherung</t>
-  </si>
-  <si>
-    <t>www.messe-essen.de</t>
-  </si>
-  <si>
     <t>www.kampmann-international.com</t>
   </si>
   <si>
     <t>www.reiseversicherung.de</t>
+  </si>
+  <si>
+    <t>Europäische Reiseversicherung AG</t>
+  </si>
+  <si>
+    <t>Lohospo GmbH</t>
+  </si>
+  <si>
+    <t>Land in Sicht AG</t>
+  </si>
+  <si>
+    <t>Logo_Kampmann.png</t>
+  </si>
+  <si>
+    <t>Logo-Datei</t>
+  </si>
+  <si>
+    <t>logo_erv.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.visualcreation.de </t>
+  </si>
+  <si>
+    <t>Logo_VC.png</t>
+  </si>
+  <si>
+    <t>Visual Creation</t>
+  </si>
+  <si>
+    <t>www.lohospo.de</t>
+  </si>
+  <si>
+    <t>Logo_Lohospo.png</t>
+  </si>
+  <si>
+    <t>www.land-in-sicht.de</t>
+  </si>
+  <si>
+    <t>Logo_LIS.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -63,6 +93,18 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -88,9 +130,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -375,7 +430,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -388,74 +443,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
       <c r="E7" s="1"/>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E26" s="1"/>
     </row>
   </sheetData>
@@ -463,6 +626,7 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
 </worksheet>

</xml_diff>

<commit_message>
add new aussteller + participants
</commit_message>
<xml_diff>
--- a/docs/aussteller.xlsx
+++ b/docs/aussteller.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Name Aussteller</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>www.messe-duesseldorf.de</t>
+  </si>
+  <si>
+    <t>BBR Verkehrstechnik</t>
+  </si>
+  <si>
+    <t>Logo_fx-Vision.png</t>
+  </si>
+  <si>
+    <t>Logo_MesseDuesseldorf.png</t>
+  </si>
+  <si>
+    <t>www.bbr-vt.de</t>
+  </si>
+  <si>
+    <t>Logo_BBR-VT.png</t>
   </si>
 </sst>
 </file>
@@ -264,38 +279,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -577,15 +585,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="A1:D32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" customWidth="1"/>
     <col min="2" max="2" width="25.109375" customWidth="1"/>
     <col min="3" max="3" width="31.88671875" customWidth="1"/>
     <col min="4" max="4" width="24.88671875" customWidth="1"/>
@@ -605,9 +613,10 @@
       <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -619,9 +628,10 @@
       <c r="D2" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -633,9 +643,10 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -647,10 +658,10 @@
       <c r="D4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="66" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -662,9 +673,10 @@
       <c r="D5" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -676,10 +688,10 @@
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -691,95 +703,100 @@
       <c r="D7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -788,172 +805,228 @@
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>15</v>
+      <c r="A16" s="1">
+        <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="8" t="s">
         <v>53</v>
       </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>16</v>
+      <c r="A17" s="1">
+        <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="8" t="s">
         <v>55</v>
       </c>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>17</v>
+      <c r="A18" s="1">
+        <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="8" t="s">
         <v>57</v>
       </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>18</v>
+      <c r="A19" s="1">
+        <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>19</v>
+      <c r="A20" s="1">
+        <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="8" t="s">
         <v>60</v>
       </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
-        <v>20</v>
+      <c r="A21" s="1">
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="11"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -976,8 +1049,9 @@
     <hyperlink ref="C12" r:id="rId17"/>
     <hyperlink ref="C13" r:id="rId18"/>
     <hyperlink ref="C9" r:id="rId19"/>
+    <hyperlink ref="C22" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>